<commit_message>
4th Test case (Create NSC)
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="132">
   <si>
     <t>UserName</t>
   </si>
@@ -406,6 +406,21 @@
   </si>
   <si>
     <t>TEST123TEST Description Test</t>
+  </si>
+  <si>
+    <t>Create New NSC</t>
+  </si>
+  <si>
+    <t>NSC Title</t>
+  </si>
+  <si>
+    <t>Test0001</t>
+  </si>
+  <si>
+    <t>2229</t>
+  </si>
+  <si>
+    <t>NSC 2229 Title Test</t>
   </si>
 </sst>
 </file>
@@ -588,6 +603,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -596,21 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="10.5"/>
@@ -950,7 +965,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -971,7 +986,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="41" t="s">
         <v>44</v>
       </c>
       <c r="L2" s="17" t="s">
@@ -982,7 +997,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="34"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -994,7 +1009,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="7"/>
-      <c r="K3" s="36"/>
+      <c r="K3" s="41"/>
       <c r="L3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +1018,7 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="34"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +1030,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="7"/>
-      <c r="K4" s="36"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1024,7 +1039,7 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="34"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="5"/>
       <c r="C5" s="9"/>
       <c r="D5" s="5"/>
@@ -1032,7 +1047,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="7"/>
-      <c r="K5" s="36"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="17" t="s">
         <v>37</v>
       </c>
@@ -1049,7 +1064,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="7"/>
-      <c r="K6" s="36"/>
+      <c r="K6" s="41"/>
       <c r="L6" s="17" t="s">
         <v>38</v>
       </c>
@@ -1078,7 +1093,7 @@
         <v>38</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="K7" s="36"/>
+      <c r="K7" s="41"/>
       <c r="L7" s="17" t="s">
         <v>39</v>
       </c>
@@ -1087,7 +1102,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="33.75">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="40" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1101,11 +1116,11 @@
       <c r="F8" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="34" t="s">
         <v>121</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="K8" s="36"/>
+      <c r="K8" s="41"/>
       <c r="L8" s="17" t="s">
         <v>40</v>
       </c>
@@ -1114,7 +1129,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="22.5">
-      <c r="A9" s="35"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
@@ -1126,7 +1141,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
-      <c r="K9" s="36"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="17" t="s">
         <v>41</v>
       </c>
@@ -1135,7 +1150,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="11.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="10" t="s">
         <v>22</v>
       </c>
@@ -1144,19 +1159,19 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="K10" s="36"/>
+      <c r="K10" s="41"/>
       <c r="L10" s="17" t="s">
         <v>42</v>
       </c>
@@ -1165,7 +1180,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
-      <c r="A11" s="35"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="12">
         <v>100000612</v>
       </c>
@@ -1174,27 +1189,27 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="38" t="s">
         <v>126</v>
       </c>
       <c r="J11" s="18"/>
-      <c r="K11" s="36"/>
+      <c r="K11" s="41"/>
       <c r="L11" s="24" t="s">
         <v>111</v>
       </c>
       <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" ht="21">
-      <c r="A12" s="35"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1204,18 +1219,18 @@
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="35" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="18"/>
-      <c r="K12" s="36"/>
+      <c r="K12" s="41"/>
       <c r="L12" s="24" t="s">
         <v>112</v>
       </c>
       <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" ht="21">
-      <c r="A13" s="35"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
@@ -1225,17 +1240,17 @@
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="41"/>
       <c r="L13" s="24" t="s">
         <v>113</v>
       </c>
       <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" ht="21">
-      <c r="A14" s="35"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
@@ -1245,14 +1260,14 @@
       <c r="D14" s="5"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="K14" s="36"/>
+      <c r="K14" s="41"/>
       <c r="L14" s="24" t="s">
         <v>114</v>
       </c>
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:13" ht="21">
-      <c r="A15" s="35"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="12" t="s">
         <v>26</v>
       </c>
@@ -1262,14 +1277,14 @@
       <c r="D15" s="5"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="K15" s="36"/>
+      <c r="K15" s="41"/>
       <c r="L15" s="24" t="s">
         <v>115</v>
       </c>
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" ht="21">
-      <c r="A16" s="35"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="12" t="s">
         <v>27</v>
       </c>
@@ -1279,13 +1294,13 @@
       <c r="D16" s="5"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
-      <c r="K16" s="36"/>
+      <c r="K16" s="41"/>
       <c r="L16" s="24" t="s">
         <v>116</v>
       </c>
       <c r="M16" s="24"/>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1">
+    <row r="17" spans="1:14" s="3" customFormat="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
@@ -1294,11 +1309,11 @@
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="36"/>
+      <c r="K17" s="41"/>
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
     </row>
-    <row r="18" spans="1:13" s="3" customFormat="1">
+    <row r="18" spans="1:14" s="3" customFormat="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -1309,7 +1324,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="1:13" s="3" customFormat="1">
+    <row r="19" spans="1:14" s="3" customFormat="1">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1336,7 +1351,7 @@
       </c>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1">
+    <row r="20" spans="1:14" s="3" customFormat="1">
       <c r="A20" s="20" t="s">
         <v>60</v>
       </c>
@@ -1360,8 +1375,18 @@
       </c>
       <c r="H20" s="24"/>
       <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1">
+      <c r="K20" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="N20" s="37"/>
+    </row>
+    <row r="21" spans="1:14" s="3" customFormat="1" ht="12.75">
       <c r="A21" s="20"/>
       <c r="B21" s="23" t="s">
         <v>61</v>
@@ -1383,9 +1408,18 @@
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1">
+      <c r="K21" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="L21" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="N21" s="38"/>
+    </row>
+    <row r="22" spans="1:14" s="3" customFormat="1">
       <c r="A22" s="20"/>
       <c r="B22" s="23" t="s">
         <v>61</v>
@@ -1407,9 +1441,14 @@
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1">
+      <c r="K22" s="8"/>
+      <c r="L22" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" ht="12.75">
       <c r="A23" s="20"/>
       <c r="B23" s="23" t="s">
         <v>61</v>
@@ -1431,9 +1470,14 @@
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1">
+      <c r="K23" s="8"/>
+      <c r="L23" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1">
       <c r="A24" s="20"/>
       <c r="B24" s="23" t="s">
         <v>61</v>
@@ -1457,7 +1501,7 @@
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1">
+    <row r="25" spans="1:14" s="3" customFormat="1">
       <c r="A25" s="20"/>
       <c r="B25" s="23" t="s">
         <v>61</v>
@@ -1481,7 +1525,7 @@
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" s="24"/>
       <c r="B26" s="23" t="s">
         <v>61</v>
@@ -1503,7 +1547,7 @@
       </c>
       <c r="H26" s="24"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:14">
       <c r="A27" s="24"/>
       <c r="B27" s="23" t="s">
         <v>61</v>
@@ -1525,7 +1569,7 @@
       </c>
       <c r="H27" s="24"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" s="24"/>
       <c r="B28" s="23" t="s">
         <v>61</v>
@@ -1547,7 +1591,7 @@
       </c>
       <c r="H28" s="24"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="A29" s="24"/>
       <c r="B29" s="23" t="s">
         <v>61</v>
@@ -1569,7 +1613,7 @@
       </c>
       <c r="H29" s="24"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" s="24"/>
       <c r="B30" s="23" t="s">
         <v>61</v>
@@ -1591,7 +1635,7 @@
       </c>
       <c r="H30" s="24"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" s="24"/>
       <c r="B31" s="23" t="s">
         <v>61</v>
@@ -1613,7 +1657,7 @@
       </c>
       <c r="H31" s="24"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" s="24"/>
       <c r="B32" s="23" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
5th Test case (Create UNSPSC)
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="137">
   <si>
     <t>UserName</t>
   </si>
@@ -421,13 +421,28 @@
   </si>
   <si>
     <t>NSC 2229 Title Test</t>
+  </si>
+  <si>
+    <t>Create New UNSPSC</t>
+  </si>
+  <si>
+    <t>UNSPSC Title</t>
+  </si>
+  <si>
+    <t>UNSPSC Description</t>
+  </si>
+  <si>
+    <t>UNSPSC123TEST</t>
+  </si>
+  <si>
+    <t>UNSPSC123TEST Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -467,6 +482,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -512,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -627,6 +648,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="10.5"/>
@@ -1310,7 +1332,9 @@
       <c r="G17" s="15"/>
       <c r="J17" s="18"/>
       <c r="K17" s="41"/>
-      <c r="L17" s="24"/>
+      <c r="L17" s="42" t="s">
+        <v>133</v>
+      </c>
       <c r="M17" s="24"/>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1">
@@ -1523,9 +1547,17 @@
       </c>
       <c r="H25" s="24"/>
       <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="K25" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="M25" s="37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="12.75">
       <c r="A26" s="24"/>
       <c r="B26" s="23" t="s">
         <v>61</v>
@@ -1546,6 +1578,15 @@
         <v>70</v>
       </c>
       <c r="H26" s="24"/>
+      <c r="K26" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="L26" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="M26" s="38" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="24"/>

</xml_diff>

<commit_message>
7th Test Case (Create Attribute)
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
   <si>
     <t>UserName</t>
   </si>
@@ -436,6 +436,15 @@
   </si>
   <si>
     <t>UNSPSC123TEST Description</t>
+  </si>
+  <si>
+    <t>Create New Attribute Group</t>
+  </si>
+  <si>
+    <t>Attr Group Name</t>
+  </si>
+  <si>
+    <t>AttrGroupTest123</t>
   </si>
 </sst>
 </file>
@@ -639,6 +648,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -648,7 +658,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,7 +941,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11:L12"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="10.5"/>
@@ -987,7 +996,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1008,7 +1017,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="42" t="s">
         <v>44</v>
       </c>
       <c r="L2" s="17" t="s">
@@ -1019,7 +1028,7 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="39"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1031,7 +1040,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="7"/>
-      <c r="K3" s="41"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="17" t="s">
         <v>19</v>
       </c>
@@ -1040,7 +1049,7 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1061,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="7"/>
-      <c r="K4" s="41"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1061,7 +1070,7 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="5"/>
       <c r="C5" s="9"/>
       <c r="D5" s="5"/>
@@ -1069,7 +1078,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="7"/>
-      <c r="K5" s="41"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="17" t="s">
         <v>37</v>
       </c>
@@ -1086,7 +1095,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="7"/>
-      <c r="K6" s="41"/>
+      <c r="K6" s="42"/>
       <c r="L6" s="17" t="s">
         <v>38</v>
       </c>
@@ -1115,7 +1124,7 @@
         <v>38</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="K7" s="41"/>
+      <c r="K7" s="42"/>
       <c r="L7" s="17" t="s">
         <v>39</v>
       </c>
@@ -1124,7 +1133,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="33.75">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="41" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1142,7 +1151,7 @@
         <v>121</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="K8" s="41"/>
+      <c r="K8" s="42"/>
       <c r="L8" s="17" t="s">
         <v>40</v>
       </c>
@@ -1151,7 +1160,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="22.5">
-      <c r="A9" s="40"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="10" t="s">
         <v>21</v>
       </c>
@@ -1163,7 +1172,7 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
-      <c r="K9" s="41"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="17" t="s">
         <v>41</v>
       </c>
@@ -1172,7 +1181,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="11.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="10" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1202,7 @@
       <c r="I10" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="K10" s="41"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="17" t="s">
         <v>42</v>
       </c>
@@ -1202,7 +1211,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
-      <c r="A11" s="40"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="12">
         <v>100000612</v>
       </c>
@@ -1224,14 +1233,14 @@
         <v>126</v>
       </c>
       <c r="J11" s="18"/>
-      <c r="K11" s="41"/>
+      <c r="K11" s="42"/>
       <c r="L11" s="24" t="s">
         <v>111</v>
       </c>
       <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" ht="21">
-      <c r="A12" s="40"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1245,14 +1254,14 @@
         <v>16</v>
       </c>
       <c r="J12" s="18"/>
-      <c r="K12" s="41"/>
+      <c r="K12" s="42"/>
       <c r="L12" s="24" t="s">
         <v>112</v>
       </c>
       <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" ht="21">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="12" t="s">
         <v>24</v>
       </c>
@@ -1265,14 +1274,14 @@
       <c r="G13" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="41"/>
+      <c r="K13" s="42"/>
       <c r="L13" s="24" t="s">
         <v>113</v>
       </c>
       <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" ht="21">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
@@ -1282,14 +1291,14 @@
       <c r="D14" s="5"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="K14" s="41"/>
+      <c r="K14" s="42"/>
       <c r="L14" s="24" t="s">
         <v>114</v>
       </c>
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:13" ht="21">
-      <c r="A15" s="40"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="12" t="s">
         <v>26</v>
       </c>
@@ -1299,14 +1308,14 @@
       <c r="D15" s="5"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="K15" s="41"/>
+      <c r="K15" s="42"/>
       <c r="L15" s="24" t="s">
         <v>115</v>
       </c>
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" ht="21">
-      <c r="A16" s="40"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="12" t="s">
         <v>27</v>
       </c>
@@ -1316,7 +1325,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
-      <c r="K16" s="41"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="24" t="s">
         <v>116</v>
       </c>
@@ -1331,8 +1340,8 @@
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="42" t="s">
+      <c r="K17" s="42"/>
+      <c r="L17" s="39" t="s">
         <v>133</v>
       </c>
       <c r="M17" s="24"/>
@@ -1631,8 +1640,14 @@
         <v>70</v>
       </c>
       <c r="H28" s="24"/>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="K28" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="12.75">
       <c r="A29" s="24"/>
       <c r="B29" s="23" t="s">
         <v>61</v>
@@ -1653,6 +1668,12 @@
         <v>70</v>
       </c>
       <c r="H29" s="24"/>
+      <c r="K29" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="L29" s="34" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="24"/>

</xml_diff>

<commit_message>
8th Test Case (Configuration/Setup INC Configuration) added
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="142">
   <si>
     <t>UserName</t>
   </si>
@@ -445,6 +445,12 @@
   </si>
   <si>
     <t>AttrGroupTest123</t>
+  </si>
+  <si>
+    <t>Setup Configuration</t>
+  </si>
+  <si>
+    <t>Attribute Group</t>
   </si>
 </sst>
 </file>
@@ -542,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -657,6 +663,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="10.5"/>
@@ -1718,8 +1730,17 @@
         <v>70</v>
       </c>
       <c r="H31" s="24"/>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="K31" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" s="44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="12.75">
       <c r="A32" s="24"/>
       <c r="B32" s="23" t="s">
         <v>61</v>
@@ -1740,6 +1761,15 @@
         <v>70</v>
       </c>
       <c r="H32" s="24"/>
+      <c r="K32" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="L32" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="M32" s="43" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="33" spans="1:11" s="32" customFormat="1" ht="42">
       <c r="A33" s="29"/>

</xml_diff>

<commit_message>
updated MCat advance search test scenario
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="191">
   <si>
     <t>UserName</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Operator</t>
   </si>
   <si>
-    <t>Test001</t>
-  </si>
-  <si>
     <t>NSC001</t>
   </si>
   <si>
@@ -399,15 +396,6 @@
     <t>INC Description</t>
   </si>
   <si>
-    <t>TEST123TEST</t>
-  </si>
-  <si>
-    <t>TEST123TEST Name Test</t>
-  </si>
-  <si>
-    <t>TEST123TEST Description Test</t>
-  </si>
-  <si>
     <t>Create New NSC</t>
   </si>
   <si>
@@ -417,12 +405,6 @@
     <t>Test0001</t>
   </si>
   <si>
-    <t>2229</t>
-  </si>
-  <si>
-    <t>NSC 2229 Title Test</t>
-  </si>
-  <si>
     <t>Create New UNSPSC</t>
   </si>
   <si>
@@ -465,7 +447,157 @@
     <t>StockCodes</t>
   </si>
   <si>
-    <t>000000021</t>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Last Stock Code Named</t>
+  </si>
+  <si>
+    <t>Last Stock Code Named From Check List</t>
+  </si>
+  <si>
+    <t>INC123TEST</t>
+  </si>
+  <si>
+    <t>INC123TEST Name Test</t>
+  </si>
+  <si>
+    <t>INC123TEST Description Test</t>
+  </si>
+  <si>
+    <t>NSC001TEST</t>
+  </si>
+  <si>
+    <t>NSC001TEST TITLE</t>
+  </si>
+  <si>
+    <t>AttrGroupTest12345</t>
+  </si>
+  <si>
+    <t>Create New Attribute</t>
+  </si>
+  <si>
+    <t>AttributeCode</t>
+  </si>
+  <si>
+    <t>AttributeName</t>
+  </si>
+  <si>
+    <t>AttrTypeId</t>
+  </si>
+  <si>
+    <t>Business Unit</t>
+  </si>
+  <si>
+    <t>01_TESTATTRCODE</t>
+  </si>
+  <si>
+    <t>TESTATTRIBUTE</t>
+  </si>
+  <si>
+    <t>Submit Assigned Item</t>
+  </si>
+  <si>
+    <t>INC NAME</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>TEST TAG</t>
+  </si>
+  <si>
+    <t>Group Detail</t>
+  </si>
+  <si>
+    <t>NSC002</t>
+  </si>
+  <si>
+    <t>CATALOGUING</t>
+  </si>
+  <si>
+    <t>TEST BU</t>
+  </si>
+  <si>
+    <t>TEST INC</t>
+  </si>
+  <si>
+    <t>Review Item</t>
+  </si>
+  <si>
+    <t>QA PENDING</t>
+  </si>
+  <si>
+    <t>TEST DA</t>
+  </si>
+  <si>
+    <t>000004481</t>
+  </si>
+  <si>
+    <t>000004499</t>
+  </si>
+  <si>
+    <t>000004523</t>
+  </si>
+  <si>
+    <t>000001446</t>
+  </si>
+  <si>
+    <t>000001529</t>
+  </si>
+  <si>
+    <t>000001552</t>
+  </si>
+  <si>
+    <t>000001594</t>
+  </si>
+  <si>
+    <t>000001636</t>
+  </si>
+  <si>
+    <t>000001305</t>
+  </si>
+  <si>
+    <t>000001313</t>
+  </si>
+  <si>
+    <t>000001339</t>
+  </si>
+  <si>
+    <t>000001362</t>
+  </si>
+  <si>
+    <t>000001370</t>
+  </si>
+  <si>
+    <t>Advance Search</t>
+  </si>
+  <si>
+    <t>000001727</t>
+  </si>
+  <si>
+    <t>000001743</t>
+  </si>
+  <si>
+    <t>000002147</t>
+  </si>
+  <si>
+    <t>000002162</t>
+  </si>
+  <si>
+    <t>000002170</t>
+  </si>
+  <si>
+    <t>000001669</t>
+  </si>
+  <si>
+    <t>000000471</t>
+  </si>
+  <si>
+    <t>000003178</t>
+  </si>
+  <si>
+    <t>000002220</t>
   </si>
 </sst>
 </file>
@@ -473,7 +605,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -522,6 +654,18 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -564,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -688,6 +832,31 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -978,16 +1147,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:P66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H28" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.125" defaultRowHeight="10.5"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="4" width="13.625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="8.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="9.875" collapsed="true"/>
     <col min="3" max="3" style="14" width="23.125" collapsed="true"/>
     <col min="4" max="4" style="4" width="23.125" collapsed="true"/>
     <col min="5" max="5" style="3" width="23.125" collapsed="true"/>
@@ -995,14 +1164,14 @@
     <col min="7" max="7" style="14" width="23.125" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="19.125" collapsed="true"/>
     <col min="9" max="9" style="4" width="23.125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="19" width="2.125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="19" width="11.375" collapsed="true"/>
     <col min="11" max="11" style="19" width="23.125" collapsed="true"/>
     <col min="12" max="16384" style="4" width="23.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -1014,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>10</v>
@@ -1026,7 +1195,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>12</v>
@@ -1036,8 +1205,8 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="46" t="s">
-        <v>18</v>
+      <c r="A2" s="55" t="s">
+        <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
@@ -1048,27 +1217,27 @@
       <c r="D2" s="5"/>
       <c r="E2" s="7"/>
       <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="K2" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="K2" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="46"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1080,16 +1249,16 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="7"/>
-      <c r="K3" s="48"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="46"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1101,16 +1270,16 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="7"/>
-      <c r="K4" s="48"/>
+      <c r="K4" s="57"/>
       <c r="L4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="46"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="5"/>
       <c r="C5" s="9"/>
       <c r="D5" s="5"/>
@@ -1118,12 +1287,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="7"/>
-      <c r="K5" s="48"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1">
@@ -1135,239 +1304,243 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="7"/>
-      <c r="K6" s="48"/>
+      <c r="K6" s="57"/>
       <c r="L6" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="K7" s="48"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="33.75">
-      <c r="A8" s="47" t="s">
-        <v>49</v>
+      <c r="A8" s="56" t="s">
+        <v>48</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="7"/>
       <c r="F8" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="K8" s="48"/>
+      <c r="H8" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="K8" s="57"/>
       <c r="L8" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="22.5">
-      <c r="A9" s="47"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
-      <c r="K9" s="48"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="11.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="7"/>
       <c r="F10" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="K10" s="48"/>
+        <v>122</v>
+      </c>
+      <c r="K10" s="57"/>
       <c r="L10" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="21">
-      <c r="A11" s="47"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="12">
         <v>100000612</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="7"/>
       <c r="F11" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="H11" s="38" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="I11" s="38" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="J11" s="18"/>
-      <c r="K11" s="48"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:13" ht="21">
-      <c r="A12" s="47"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J12" s="18"/>
-      <c r="K12" s="48"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:13" ht="21">
-      <c r="A13" s="47"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="48"/>
+        <v>14</v>
+      </c>
+      <c r="K13" s="57"/>
       <c r="L13" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M13" s="24"/>
     </row>
     <row r="14" spans="1:13" ht="21">
-      <c r="A14" s="47"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="K14" s="48"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="24" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M14" s="24"/>
     </row>
     <row r="15" spans="1:13" ht="21">
-      <c r="A15" s="47"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="K15" s="48"/>
+      <c r="K15" s="57"/>
       <c r="L15" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:13" ht="21">
-      <c r="A16" s="47"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
-      <c r="K16" s="48"/>
+      <c r="K16" s="57"/>
       <c r="L16" s="24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M16" s="24"/>
     </row>
@@ -1380,9 +1553,9 @@
       <c r="F17" s="8"/>
       <c r="G17" s="15"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="48"/>
+      <c r="K17" s="57"/>
       <c r="L17" s="39" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M17" s="24"/>
     </row>
@@ -1399,25 +1572,25 @@
     </row>
     <row r="19" spans="1:14" s="3" customFormat="1">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>8</v>
@@ -1426,97 +1599,97 @@
     </row>
     <row r="20" spans="1:14" s="3" customFormat="1">
       <c r="A20" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="24" t="s">
+      <c r="G20" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>70</v>
       </c>
       <c r="H20" s="24"/>
       <c r="J20" s="18"/>
       <c r="K20" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="1:14" s="3" customFormat="1" ht="12.75">
+    <row r="21" spans="1:14" s="3" customFormat="1">
       <c r="A21" s="20"/>
       <c r="B21" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>72</v>
-      </c>
       <c r="F21" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H21" s="24"/>
       <c r="J21" s="18"/>
       <c r="K21" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="L21" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="M21" s="38" t="s">
-        <v>131</v>
+        <v>123</v>
+      </c>
+      <c r="L21" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="M21" s="49" t="s">
+        <v>147</v>
       </c>
       <c r="N21" s="38"/>
     </row>
     <row r="22" spans="1:14" s="3" customFormat="1">
       <c r="A22" s="20"/>
       <c r="B22" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>74</v>
-      </c>
       <c r="F22" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H22" s="24"/>
       <c r="J22" s="18"/>
       <c r="K22" s="8"/>
       <c r="L22" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -1524,28 +1697,28 @@
     <row r="23" spans="1:14" s="3" customFormat="1" ht="12.75">
       <c r="A23" s="20"/>
       <c r="B23" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>76</v>
-      </c>
       <c r="F23" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H23" s="24"/>
       <c r="J23" s="18"/>
       <c r="K23" s="8"/>
       <c r="L23" s="34" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -1553,22 +1726,22 @@
     <row r="24" spans="1:14" s="3" customFormat="1">
       <c r="A24" s="20"/>
       <c r="B24" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>78</v>
-      </c>
       <c r="F24" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H24" s="24"/>
       <c r="J24" s="18"/>
@@ -1577,456 +1750,689 @@
     <row r="25" spans="1:14" s="3" customFormat="1">
       <c r="A25" s="20"/>
       <c r="B25" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="24" t="s">
-        <v>80</v>
-      </c>
       <c r="F25" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="24"/>
       <c r="J25" s="18"/>
       <c r="K25" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="12.75">
       <c r="A26" s="24"/>
       <c r="B26" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>82</v>
-      </c>
       <c r="F26" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H26" s="24"/>
       <c r="K26" s="36" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L26" s="34" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="M26" s="38" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="24"/>
       <c r="B27" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>84</v>
-      </c>
       <c r="F27" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H27" s="24"/>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="24"/>
       <c r="B28" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>86</v>
-      </c>
       <c r="F28" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H28" s="24"/>
       <c r="K28" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="12.75">
       <c r="A29" s="24"/>
       <c r="B29" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>88</v>
-      </c>
       <c r="F29" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H29" s="24"/>
       <c r="K29" s="36" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="L29" s="34" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="24"/>
       <c r="B30" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>90</v>
-      </c>
       <c r="F30" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="24"/>
       <c r="B31" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>92</v>
-      </c>
       <c r="F31" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H31" s="24"/>
       <c r="K31" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L31" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M31" s="41" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="12.75">
       <c r="A32" s="24"/>
       <c r="B32" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>94</v>
-      </c>
       <c r="F32" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H32" s="24"/>
       <c r="K32" s="36" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="L32" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M32" s="40" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A33" s="29"/>
       <c r="B33" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="D33" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="E33" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="F33" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="26" t="s">
         <v>98</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="G33" s="26" t="s">
-        <v>99</v>
       </c>
       <c r="H33" s="29"/>
       <c r="J33" s="33"/>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" spans="1:15" s="32" customFormat="1" ht="42">
+    <row r="34" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A34" s="29"/>
       <c r="B34" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D34" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="29" t="s">
-        <v>101</v>
-      </c>
       <c r="F34" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H34" s="29"/>
       <c r="J34" s="33"/>
       <c r="K34" s="42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L34" s="42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M34" s="43" t="s">
         <v>0</v>
       </c>
       <c r="N34" s="43" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="O34" s="43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A35" s="29"/>
       <c r="B35" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D35" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E35" s="29" t="s">
-        <v>103</v>
-      </c>
       <c r="F35" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H35" s="29"/>
       <c r="J35" s="33"/>
       <c r="K35" s="44" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="L35" s="34" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M35" s="45" t="s">
         <v>2</v>
       </c>
       <c r="N35" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="O35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A36" s="29"/>
       <c r="B36" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D36" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="29" t="s">
-        <v>105</v>
-      </c>
       <c r="F36" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H36" s="29"/>
       <c r="J36" s="33"/>
       <c r="K36" s="33"/>
+      <c r="L36" s="32" t="s">
+        <v>162</v>
+      </c>
       <c r="O36" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A37" s="29"/>
       <c r="B37" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D37" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>107</v>
-      </c>
       <c r="F37" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H37" s="29"/>
       <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
+      <c r="K37" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="O37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A38" s="29"/>
       <c r="B38" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D38" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H38" s="29"/>
       <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
+      <c r="K38" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="L38" t="s">
+        <v>190</v>
+      </c>
       <c r="O38" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" s="32" customFormat="1" ht="42">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A39" s="29"/>
       <c r="B39" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D39" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F39" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H39" s="29"/>
       <c r="J39" s="33"/>
       <c r="K39" s="33"/>
     </row>
-    <row r="40" spans="1:15" s="32" customFormat="1" ht="42">
+    <row r="40" spans="1:16" s="32" customFormat="1" ht="42">
       <c r="A40" s="29"/>
       <c r="B40" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="29" t="s">
-        <v>96</v>
-      </c>
       <c r="D40" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H40" s="29"/>
       <c r="J40" s="33"/>
       <c r="K40" s="33"/>
+    </row>
+    <row r="43" spans="1:16" ht="31.5">
+      <c r="A43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="H43" s="53" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="K43" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="L43" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="M43" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="N43" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="O43" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="P43" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="12.75">
+      <c r="A44" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="51" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="H44" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="J44" t="s">
+        <v>171</v>
+      </c>
+      <c r="K44" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="L44" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="M44" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="N44" t="s">
+        <v>167</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="C45" s="48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="12.75">
+      <c r="C46" s="48"/>
+      <c r="J46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="12.75">
+      <c r="C47" s="48"/>
+      <c r="E47" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="J47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="12.75">
+      <c r="C48" s="48"/>
+      <c r="E48" t="s">
+        <v>176</v>
+      </c>
+      <c r="F48" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="J48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" ht="12.75">
+      <c r="C49" s="48"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="4"/>
+      <c r="J49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" ht="12.75">
+      <c r="C50" s="48"/>
+      <c r="E50" t="s">
+        <v>177</v>
+      </c>
+      <c r="F50" s="19"/>
+      <c r="G50" s="4"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="3:10" ht="12.75">
+      <c r="C51" s="48"/>
+      <c r="E51" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" s="19"/>
+      <c r="G51" s="4"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="3:10" ht="12.75">
+      <c r="C52" s="48"/>
+      <c r="E52" t="s">
+        <v>179</v>
+      </c>
+      <c r="F52" s="19"/>
+      <c r="G52" s="4"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="3:10" ht="12.75">
+      <c r="C53" s="48"/>
+      <c r="E53" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="4"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="3:10" ht="12.75">
+      <c r="C54" s="48"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="3:10" ht="12.75">
+      <c r="C55" s="48"/>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="3:10" ht="12.75">
+      <c r="C56" s="48"/>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="3:10" ht="12.75">
+      <c r="C57" s="48"/>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="3:10" ht="12.75">
+      <c r="C58" s="48"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="3:10" ht="12.75">
+      <c r="C59" s="48"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="3:10" ht="12.75">
+      <c r="C60" s="48"/>
+      <c r="J60"/>
+    </row>
+    <row r="61" spans="3:10">
+      <c r="C61" s="48"/>
+    </row>
+    <row r="62" spans="3:10">
+      <c r="C62" s="48"/>
+    </row>
+    <row r="63" spans="3:10">
+      <c r="C63" s="48"/>
+    </row>
+    <row r="64" spans="3:10">
+      <c r="C64" s="48"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="48"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2051,16 +2457,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>